<commit_message>
added cleaned-up tables for paper submission
</commit_message>
<xml_diff>
--- a/tables/table1.xlsx
+++ b/tables/table1.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="27960" windowHeight="18520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -166,8 +171,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +184,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -219,12 +230,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,15 +538,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="4" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="11" width="13.5" customWidth="1"/>
+    <col min="12" max="12" width="19.5" customWidth="1"/>
+    <col min="13" max="13" width="17.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -569,10 +604,10 @@
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -610,10 +645,10 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -651,10 +686,10 @@
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -692,10 +727,10 @@
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -729,14 +764,14 @@
         <v>0.97</v>
       </c>
       <c r="M6" s="2">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -770,14 +805,14 @@
         <v>0.97</v>
       </c>
       <c r="M7" s="2">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -815,10 +850,10 @@
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -856,10 +891,10 @@
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -896,11 +931,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:13" ht="28">
+      <c r="A11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -934,14 +969,14 @@
         <v>0.97</v>
       </c>
       <c r="M11" s="2">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="1" t="s">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="28">
+      <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -975,14 +1010,14 @@
         <v>0.97</v>
       </c>
       <c r="M12" s="2">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="1" t="s">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="50" customHeight="1">
+      <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1016,14 +1051,14 @@
         <v>0.82</v>
       </c>
       <c r="M13" s="2">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="1" t="s">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="50" customHeight="1">
+      <c r="A14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1057,14 +1092,14 @@
         <v>0.97</v>
       </c>
       <c r="M14" s="2">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="1" t="s">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="50" customHeight="1">
+      <c r="A15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1098,14 +1133,14 @@
         <v>0.82</v>
       </c>
       <c r="M15" s="2">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="1" t="s">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="50" customHeight="1">
+      <c r="A16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1139,14 +1174,14 @@
         <v>0.97</v>
       </c>
       <c r="M16" s="2">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="1" t="s">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="50" customHeight="1">
+      <c r="A17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1184,6 +1219,13 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="53" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>